<commit_message>
added definition for half of the columns.
</commit_message>
<xml_diff>
--- a/SF_Plan.xlsx
+++ b/SF_Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitnverma/Desktop/2020-2021-2022/Parsh/ScienceFair/GHG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parshverma/Desktop/sciencefair/sciencefair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDDB08D-828B-DB44-8523-E71FC3A55BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88384DF9-F4A8-A742-9315-E78F1B6995E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" firstSheet="3" activeTab="4" xr2:uid="{412144E9-6F29-48AA-9BCA-3BBECBC8B2AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19120" firstSheet="3" activeTab="4" xr2:uid="{412144E9-6F29-48AA-9BCA-3BBECBC8B2AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Migration Planning" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="462">
   <si>
     <t>Task #</t>
   </si>
@@ -1417,9 +1417,6 @@
     <t>Require levelling?</t>
   </si>
   <si>
-    <t>List</t>
-  </si>
-  <si>
     <t>Cardinality(H/M/L)</t>
   </si>
   <si>
@@ -1470,6 +1467,27 @@
   </si>
   <si>
     <t>Acceptable Values</t>
+  </si>
+  <si>
+    <t>List of Strings</t>
+  </si>
+  <si>
+    <t>Discrete</t>
+  </si>
+  <si>
+    <t>FDI: Foreign Direct Investment. Investments made by a company or governement into a foreign concern. FDI Inflows are the investments that come into the nation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The annual growth rate is the rate at which the nations GDP changes. It is also described as the measurment of the increase in value of a revenue stream in a given year. This rate is used to measure a nations economy(determining wether it is in recession or expansion). </t>
+  </si>
+  <si>
+    <t>The ratio of people primarily depending on clean fuels for certain task to the total amount of people that perform that task.</t>
+  </si>
+  <si>
+    <t>Ratio of number of deaths in the year to the average total population. Esentially Death Rate</t>
+  </si>
+  <si>
+    <t>What percent/ratio of the total consumption of energy in a nation is renewable. Ex. In the U.S. renewable energy generates 20% of the U.S electricity.</t>
   </si>
 </sst>
 </file>
@@ -1973,14 +1991,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="107">
+  <dxfs count="93">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <u val="none"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2043,143 +2064,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkVertical">
-          <fgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkVertical">
-          <fgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2859,11 +2743,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEEB311-16E5-744C-8EC1-E109AF370A0D}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FEEB311-16E5-744C-8EC1-E109AF370A0D}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A77117F1-CCBD-B345-BC47-9B71C5B6B988}" name="Task" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{49E712B1-6EAC-2843-B035-DE32AF8B9C3A}" name="Description" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{6786B55A-B298-EF4C-A543-988B38B701D4}" name="Progress Notes" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{A77117F1-CCBD-B345-BC47-9B71C5B6B988}" name="Task" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{49E712B1-6EAC-2843-B035-DE32AF8B9C3A}" name="Description" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{6786B55A-B298-EF4C-A543-988B38B701D4}" name="Progress Notes" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4930,299 +4814,299 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:C14">
-    <cfRule type="expression" dxfId="106" priority="97">
+    <cfRule type="expression" dxfId="92" priority="97">
       <formula>$Q14="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="98">
+    <cfRule type="expression" dxfId="91" priority="98">
       <formula>$Q14=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="99">
+    <cfRule type="expression" dxfId="90" priority="99">
       <formula>AND($Q14&lt;&gt;"Completed",$Q14&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4">
-    <cfRule type="expression" dxfId="103" priority="94">
+    <cfRule type="expression" dxfId="89" priority="94">
       <formula>$Q4="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="95">
+    <cfRule type="expression" dxfId="88" priority="95">
       <formula>$Q4=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="96">
+    <cfRule type="expression" dxfId="87" priority="96">
       <formula>AND($Q4&lt;&gt;"Completed",$Q4&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C17">
-    <cfRule type="expression" dxfId="100" priority="91">
+    <cfRule type="expression" dxfId="86" priority="91">
       <formula>$Q17="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="92">
+    <cfRule type="expression" dxfId="85" priority="92">
       <formula>$Q17=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="93">
+    <cfRule type="expression" dxfId="84" priority="93">
       <formula>AND($Q17&lt;&gt;"Completed",$Q17&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:C26">
-    <cfRule type="expression" dxfId="97" priority="88">
+    <cfRule type="expression" dxfId="83" priority="88">
       <formula>$Q26="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="89">
+    <cfRule type="expression" dxfId="82" priority="89">
       <formula>$Q26=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="90">
+    <cfRule type="expression" dxfId="81" priority="90">
       <formula>AND($Q26&lt;&gt;"Completed",$Q26&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:C39">
-    <cfRule type="expression" dxfId="94" priority="82">
+    <cfRule type="expression" dxfId="80" priority="82">
       <formula>$Q39="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="83">
+    <cfRule type="expression" dxfId="79" priority="83">
       <formula>$Q39=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="84">
+    <cfRule type="expression" dxfId="78" priority="84">
       <formula>AND($Q39&lt;&gt;"Completed",$Q39&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C22">
-    <cfRule type="expression" dxfId="91" priority="79">
+    <cfRule type="expression" dxfId="77" priority="79">
       <formula>$Q22="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="80">
+    <cfRule type="expression" dxfId="76" priority="80">
       <formula>$Q22=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="81">
+    <cfRule type="expression" dxfId="75" priority="81">
       <formula>AND($Q22&lt;&gt;"Completed",$Q22&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53:C53">
-    <cfRule type="expression" dxfId="88" priority="76">
+    <cfRule type="expression" dxfId="74" priority="76">
       <formula>$Q53="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="77">
+    <cfRule type="expression" dxfId="73" priority="77">
       <formula>$Q53=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="78">
+    <cfRule type="expression" dxfId="72" priority="78">
       <formula>AND($Q53&lt;&gt;"Completed",$Q53&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:C61">
-    <cfRule type="expression" dxfId="85" priority="73">
+    <cfRule type="expression" dxfId="71" priority="73">
       <formula>$Q61="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="74">
+    <cfRule type="expression" dxfId="70" priority="74">
       <formula>$Q61=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="75">
+    <cfRule type="expression" dxfId="69" priority="75">
       <formula>AND($Q61&lt;&gt;"Completed",$Q61&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70:C70">
-    <cfRule type="expression" dxfId="82" priority="70">
+    <cfRule type="expression" dxfId="68" priority="70">
       <formula>$Q70="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71">
+    <cfRule type="expression" dxfId="67" priority="71">
       <formula>$Q70=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="72">
+    <cfRule type="expression" dxfId="66" priority="72">
       <formula>AND($Q70&lt;&gt;"Completed",$Q70&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:C75">
-    <cfRule type="expression" dxfId="79" priority="67">
+    <cfRule type="expression" dxfId="65" priority="67">
       <formula>$Q75="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="68">
+    <cfRule type="expression" dxfId="64" priority="68">
       <formula>$Q75=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="69">
+    <cfRule type="expression" dxfId="63" priority="69">
       <formula>AND($Q75&lt;&gt;"Completed",$Q75&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:C121">
-    <cfRule type="expression" dxfId="76" priority="55">
+    <cfRule type="expression" dxfId="62" priority="55">
       <formula>$Q122="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="56">
+    <cfRule type="expression" dxfId="61" priority="56">
       <formula>$Q122=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="57">
+    <cfRule type="expression" dxfId="60" priority="57">
       <formula>AND($Q122&lt;&gt;"Completed",$Q122&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B148:C148">
-    <cfRule type="expression" dxfId="73" priority="46">
+    <cfRule type="expression" dxfId="59" priority="46">
       <formula>$Q149="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="47">
+    <cfRule type="expression" dxfId="58" priority="47">
       <formula>$Q149=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="48">
+    <cfRule type="expression" dxfId="57" priority="48">
       <formula>AND($Q149&lt;&gt;"Completed",$Q149&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B153:C153">
-    <cfRule type="expression" dxfId="70" priority="43">
+    <cfRule type="expression" dxfId="56" priority="43">
       <formula>$Q154="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="44">
+    <cfRule type="expression" dxfId="55" priority="44">
       <formula>$Q154=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="45">
+    <cfRule type="expression" dxfId="54" priority="45">
       <formula>AND($Q154&lt;&gt;"Completed",$Q154&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B156:C156">
-    <cfRule type="expression" dxfId="67" priority="40">
+    <cfRule type="expression" dxfId="53" priority="40">
       <formula>$Q157="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="41">
+    <cfRule type="expression" dxfId="52" priority="41">
       <formula>$Q157=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="42">
+    <cfRule type="expression" dxfId="51" priority="42">
       <formula>AND($Q157&lt;&gt;"Completed",$Q157&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B159:C159">
-    <cfRule type="expression" dxfId="64" priority="37">
+    <cfRule type="expression" dxfId="50" priority="37">
       <formula>$Q160="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="38">
+    <cfRule type="expression" dxfId="49" priority="38">
       <formula>$Q160=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="39">
+    <cfRule type="expression" dxfId="48" priority="39">
       <formula>AND($Q160&lt;&gt;"Completed",$Q160&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B178:C178">
-    <cfRule type="expression" dxfId="61" priority="34">
+    <cfRule type="expression" dxfId="47" priority="34">
       <formula>$Q179="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="35">
+    <cfRule type="expression" dxfId="46" priority="35">
       <formula>$Q179=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="36">
+    <cfRule type="expression" dxfId="45" priority="36">
       <formula>AND($Q179&lt;&gt;"Completed",$Q179&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B197:C197">
-    <cfRule type="expression" dxfId="58" priority="31">
+    <cfRule type="expression" dxfId="44" priority="31">
       <formula>$Q198="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="32">
+    <cfRule type="expression" dxfId="43" priority="32">
       <formula>$Q198=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="33">
+    <cfRule type="expression" dxfId="42" priority="33">
       <formula>AND($Q198&lt;&gt;"Completed",$Q198&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B200:C200">
-    <cfRule type="expression" dxfId="55" priority="28">
+    <cfRule type="expression" dxfId="41" priority="28">
       <formula>$Q202="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="29">
+    <cfRule type="expression" dxfId="40" priority="29">
       <formula>$Q202=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="30">
+    <cfRule type="expression" dxfId="39" priority="30">
       <formula>AND($Q202&lt;&gt;"Completed",$Q202&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="expression" dxfId="52" priority="25">
+    <cfRule type="expression" dxfId="38" priority="25">
       <formula>$Q29="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="26">
+    <cfRule type="expression" dxfId="37" priority="26">
       <formula>$Q29=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="27">
+    <cfRule type="expression" dxfId="36" priority="27">
       <formula>AND($Q29&lt;&gt;"Completed",$Q29&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:C46 B51:C51">
-    <cfRule type="expression" dxfId="49" priority="22">
+    <cfRule type="expression" dxfId="35" priority="22">
       <formula>$Q46="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="23">
+    <cfRule type="expression" dxfId="34" priority="23">
       <formula>$Q46=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="24">
+    <cfRule type="expression" dxfId="33" priority="24">
       <formula>AND($Q46&lt;&gt;"Completed",$Q46&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B131:C131">
-    <cfRule type="expression" dxfId="46" priority="19">
+    <cfRule type="expression" dxfId="32" priority="19">
       <formula>$Q132="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="20">
+    <cfRule type="expression" dxfId="31" priority="20">
       <formula>$Q132=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="21">
+    <cfRule type="expression" dxfId="30" priority="21">
       <formula>AND($Q132&lt;&gt;"Completed",$Q132&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138:C138">
-    <cfRule type="expression" dxfId="43" priority="16">
+    <cfRule type="expression" dxfId="29" priority="16">
       <formula>$Q139="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="17">
+    <cfRule type="expression" dxfId="28" priority="17">
       <formula>$Q139=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="18">
+    <cfRule type="expression" dxfId="27" priority="18">
       <formula>AND($Q139&lt;&gt;"Completed",$Q139&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="expression" dxfId="40" priority="13">
+    <cfRule type="expression" dxfId="26" priority="13">
       <formula>$Q144="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="14">
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>$Q144=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="15">
+    <cfRule type="expression" dxfId="24" priority="15">
       <formula>AND($Q144&lt;&gt;"Completed",$Q144&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C143">
-    <cfRule type="expression" dxfId="37" priority="10">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>$Q144="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="11">
+    <cfRule type="expression" dxfId="22" priority="11">
       <formula>$Q144=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="12">
+    <cfRule type="expression" dxfId="21" priority="12">
       <formula>AND($Q144&lt;&gt;"Completed",$Q144&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="expression" dxfId="34" priority="7">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>$Q118="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="8">
+    <cfRule type="expression" dxfId="19" priority="8">
       <formula>$Q118=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="9">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>AND($Q118&lt;&gt;"Completed",$Q118&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C117">
-    <cfRule type="expression" dxfId="31" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>$Q142="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>$Q142=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>AND($Q142&lt;&gt;"Completed",$Q142&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:C32">
-    <cfRule type="expression" dxfId="28" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$Q32="Completed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$Q32=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>AND($Q32&lt;&gt;"Completed",$Q32&lt;&gt;" ")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8214,37 +8098,37 @@
   <autoFilter ref="A1:I27" xr:uid="{C3C3D8AF-82D6-6A4E-9A8F-7EA23972EFF6}"/>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="L1:CM1">
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>WEEKDAY(L$1,2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4:CM7 L18:CM20">
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(L$1&gt;=$F7,L$1&lt;=$G7,$F5="Completed")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B27 A19:H23 D26:H27 A15:H17 A3:H13">
-    <cfRule type="expression" dxfId="11" priority="107">
+    <cfRule type="expression" dxfId="4" priority="107">
       <formula>$H3="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C27">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$H25="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:CM35">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(L$1&gt;=$F3,L$1&lt;=$G3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$H35="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G61">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($G3&lt;TODAY(),$G3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8260,7 +8144,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="B88" sqref="B7:B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8291,16 +8175,16 @@
         <v>421</v>
       </c>
       <c r="E1" s="88" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F1" s="88" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G1" s="88" t="s">
         <v>439</v>
       </c>
       <c r="H1" s="88" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I1" s="88" t="s">
         <v>6</v>
@@ -8308,38 +8192,38 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="91" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="91" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F3" s="93"/>
       <c r="H3" s="93"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="91" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E4" s="90" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="91" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="91" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F6" s="90" t="s">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="H6" s="93" t="s">
         <v>438</v>
@@ -8353,7 +8237,10 @@
         <v>420</v>
       </c>
       <c r="D7" s="90" t="s">
-        <v>449</v>
+        <v>448</v>
+      </c>
+      <c r="F7" s="90" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="136" x14ac:dyDescent="0.2">
@@ -8361,39 +8248,54 @@
         <v>424</v>
       </c>
       <c r="B8" s="92" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D8" s="90" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H8" s="92"/>
       <c r="I8" s="92" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="91" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="92" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="91" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="92" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="91" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="92" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="91" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="92" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="91" t="s">
         <v>429</v>
+      </c>
+      <c r="B13" s="92" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -8416,7 +8318,7 @@
         <v>433</v>
       </c>
       <c r="F17" s="90" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H17" s="90">
         <v>1</v>
@@ -8448,6 +8350,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072CC0728E1A7344696CB36879E6DD8AF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bc41760786a4b448dc5958478ca8ab2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29649c66-3e48-49a8-b9d2-7f9225ba445b" xmlns:ns3="f28237a1-9120-4872-aa74-abd7e45fa072" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa0647d0b64366ab1344d974d2175da6" ns2:_="" ns3:_="">
     <xsd:import namespace="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
@@ -8670,17 +8583,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8691,6 +8593,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09320F3B-B84A-40C1-951B-A3CEB4621E81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8709,23 +8628,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7047B261-B032-4F38-845E-538EC0EF3CE9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added description for half of the columns
</commit_message>
<xml_diff>
--- a/SF_Plan.xlsx
+++ b/SF_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parshverma/Desktop/sciencefair/sciencefair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88384DF9-F4A8-A742-9315-E78F1B6995E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EC1DA8-049A-244D-9CBB-51055FE18299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19120" firstSheet="3" activeTab="4" xr2:uid="{412144E9-6F29-48AA-9BCA-3BBECBC8B2AE}"/>
   </bookViews>
@@ -8141,10 +8141,10 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B88" sqref="B7:B88"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8350,17 +8350,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072CC0728E1A7344696CB36879E6DD8AF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bc41760786a4b448dc5958478ca8ab2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29649c66-3e48-49a8-b9d2-7f9225ba445b" xmlns:ns3="f28237a1-9120-4872-aa74-abd7e45fa072" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa0647d0b64366ab1344d974d2175da6" ns2:_="" ns3:_="">
     <xsd:import namespace="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
@@ -8583,6 +8572,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8593,23 +8593,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09320F3B-B84A-40C1-951B-A3CEB4621E81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8628,6 +8611,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7047B261-B032-4F38-845E-538EC0EF3CE9}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
finished writing definitions for columns
finished writing definitions for columns
</commit_message>
<xml_diff>
--- a/SF_Plan.xlsx
+++ b/SF_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parshverma/Desktop/sciencefair/sciencefair/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631AC642-BDE6-B641-8272-CF2EE8496748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C978B4CE-87BD-4144-97BB-690192CED144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19940" firstSheet="3" activeTab="4" xr2:uid="{412144E9-6F29-48AA-9BCA-3BBECBC8B2AE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="473">
   <si>
     <t>Task #</t>
   </si>
@@ -1494,6 +1494,57 @@
 creating a new dataframe
 2. Data cleaning imputation</t>
   </si>
+  <si>
+    <t>CO2 emission(Metric tons per capita)Carbon dioxide emissions are those stemming from the burning of fossil fuels and the manufacture of cement. They include carbon dioxide produced during consumption of solid, liquid, and gas fuels and gas flaring.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A fossil fuel subsidy is any government action that lowers the cost of fossil fuel energy production, raises the price received by energy producers, or lowers the price paid by energy consumers.Subsidies have sizable fiscal costs (leading to higher taxes/borrowing or lower spending), promote inefficient allocation of an economy’s resources (hindering growth), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">encourage pollution </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(contributing to climate change and premature deaths from local air pollution), and are not well targeted at the poor (mostly benefiting higher income households). </t>
+    </r>
+  </si>
+  <si>
+    <t>Research and development (R&amp;D) expenses are direct expenditures relating to a company's/country's efforts to develop, design, and enhance its products, services, technologies, or processes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Countries recognized the need for specific climate financing in the Paris Agreement which calls for “making finance flows consistent with a pathway towards low greenhouse gas emissions and climate-resilient development. </t>
+  </si>
+  <si>
+    <t>92% of S&amp;P 500® Companies and 70% of Russell 1000® Companies Published Sustainability Reports in 2020, G&amp;A Institute Research Shows.</t>
+  </si>
+  <si>
+    <t>Education for Sustainable Development means including key sustainable development issues into teaching and learning; for example, climate change, disaster risk reduction, biodiversity, poverty reduction, and sustainable consumption.</t>
+  </si>
+  <si>
+    <t>The 2030 Agenda commits the global community to “achieving sustainable development in its three dimensions—economic, social and environmental—in a balanced and integrated manner”.The Global Goals and the 2030 Agenda for Sustainable Development seek to end poverty and hunger, realise the human rights of all, achieve gender equality and the empowerment of all women and girls, and ensure the lasting protection of the planet and its natural resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land degradation is defined as the reduction or loss of the biological or economic productivity and complexity of rain fed cropland, irrigated cropland, or range, pasture, forest and woodlands resulting from a combination of pressures, including land use and management practices. </t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
 </sst>
 </file>
 
@@ -1503,7 +1554,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1636,6 +1687,56 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1758,10 +1859,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1995,8 +2097,24 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="93">
@@ -8149,10 +8267,10 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8241,7 +8359,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="136" x14ac:dyDescent="0.2">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="97" t="s">
         <v>423</v>
       </c>
       <c r="B7" s="92" t="s">
@@ -8254,8 +8372,8 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="A8" s="91" t="s">
+    <row r="8" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A8" s="95" t="s">
         <v>424</v>
       </c>
       <c r="B8" s="92" t="s">
@@ -8270,7 +8388,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="95" t="s">
         <v>425</v>
       </c>
       <c r="B9" s="92" t="s">
@@ -8309,58 +8427,107 @@
         <v>460</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="91" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="92" t="s">
+        <v>463</v>
+      </c>
+      <c r="I14" s="98" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="91" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="92" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="91" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="92" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="91" t="s">
         <v>433</v>
       </c>
+      <c r="B17" s="92" t="s">
+        <v>466</v>
+      </c>
       <c r="F17" s="90" t="s">
         <v>445</v>
       </c>
       <c r="H17" s="90">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="98" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="91" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="92" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="91" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="91" t="s">
+      <c r="B19" s="92" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="96" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="92" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="52" x14ac:dyDescent="0.25">
       <c r="A21" s="91" t="s">
         <v>437</v>
       </c>
+      <c r="B21" s="92" t="s">
+        <v>470</v>
+      </c>
+      <c r="I21" s="99" t="s">
+        <v>472</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I14" r:id="rId1" xr:uid="{558F3624-11C9-9947-87B3-24CCE3CB526D}"/>
+    <hyperlink ref="I17" r:id="rId2" xr:uid="{6C9D4966-43FD-8049-8ACD-A9384890B1BF}"/>
+    <hyperlink ref="I21" r:id="rId3" xr:uid="{370B8DB7-EC7A-0E45-B988-5FCEC700A4F2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072CC0728E1A7344696CB36879E6DD8AF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bc41760786a4b448dc5958478ca8ab2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29649c66-3e48-49a8-b9d2-7f9225ba445b" xmlns:ns3="f28237a1-9120-4872-aa74-abd7e45fa072" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa0647d0b64366ab1344d974d2175da6" ns2:_="" ns3:_="">
     <xsd:import namespace="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
@@ -8583,17 +8750,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="29649c66-3e48-49a8-b9d2-7f9225ba445b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f28237a1-9120-4872-aa74-abd7e45fa072" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8604,6 +8760,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09320F3B-B84A-40C1-951B-A3CEB4621E81}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8622,23 +8795,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7068443-845F-4554-802D-AB17D3A78DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29649c66-3e48-49a8-b9d2-7f9225ba445b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f28237a1-9120-4872-aa74-abd7e45fa072"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7047B261-B032-4F38-845E-538EC0EF3CE9}">
   <ds:schemaRefs>

</xml_diff>